<commit_message>
part of storeItemDefine rebuild
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>level</t>
+    <t>title</t>
   </si>
   <si>
     <t>equipType</t>
@@ -44,10 +44,7 @@
     <t>equipClass</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>iconResource</t>
+    <t>isExpendable</t>
   </si>
   <si>
     <t>equipResource</t>
@@ -65,6 +62,9 @@
     <t>effect1.invokeType</t>
   </si>
   <si>
+    <t>effect1.invokeNum</t>
+  </si>
+  <si>
     <t>effect1.propertyType</t>
   </si>
   <si>
@@ -80,6 +80,9 @@
     <t>effect2.invokeType</t>
   </si>
   <si>
+    <t>effect2.invokeNum</t>
+  </si>
+  <si>
     <t>effect2.propertyType</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
     <t>effect3.invokeType</t>
   </si>
   <si>
+    <t>effect3.invokeNum</t>
+  </si>
+  <si>
     <t>effect3.propertyType</t>
   </si>
   <si>
@@ -104,220 +110,112 @@
     <t>effect3.value</t>
   </si>
   <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>ExtraEntry1</t>
-  </si>
-  <si>
-    <t>ExtraEntry2</t>
-  </si>
-  <si>
-    <t>ExtraEntry3</t>
-  </si>
-  <si>
     <t>wood_sword</t>
   </si>
   <si>
-    <t>wood_sword_icon</t>
-  </si>
-  <si>
     <t>wood_sword_icon_big</t>
   </si>
   <si>
-    <t>wood_sword吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>iron_sword</t>
   </si>
   <si>
-    <t>iron_sword_icon</t>
-  </si>
-  <si>
     <t>iron_sword_icon_big</t>
   </si>
   <si>
-    <t>iron_sword吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>magic_sword</t>
   </si>
   <si>
-    <t>magic_sword_icon</t>
-  </si>
-  <si>
     <t>magic_sword_icon_big</t>
   </si>
   <si>
-    <t>magic_sword吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>fast_shoes</t>
   </si>
   <si>
-    <t>fast_shoes_icon</t>
-  </si>
-  <si>
     <t>fast_shoes_icon_big</t>
   </si>
   <si>
-    <t>fast_shoes吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>stab_shield</t>
   </si>
   <si>
-    <t>stab_shield_icon</t>
-  </si>
-  <si>
     <t>stab_shield_icon_big</t>
   </si>
   <si>
-    <t>stab_shield吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>arm_shield</t>
   </si>
   <si>
-    <t>arm_shield_icon</t>
-  </si>
-  <si>
     <t>arm_shield_icon_big</t>
   </si>
   <si>
-    <t>arm_shield吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>wood_shield</t>
   </si>
   <si>
-    <t>wood_shield_icon</t>
-  </si>
-  <si>
     <t>wood_shield_icon_big</t>
   </si>
   <si>
-    <t>wood_shield吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>long_arch</t>
   </si>
   <si>
-    <t>long_arch_icon</t>
-  </si>
-  <si>
     <t>long_arch_icon_big</t>
   </si>
   <si>
-    <t>long_arch吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>wood_arch</t>
   </si>
   <si>
-    <t>wood_arch_icon</t>
-  </si>
-  <si>
     <t>wood_arch_icon_big</t>
   </si>
   <si>
-    <t>wood_arch吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>zhuge_bow</t>
   </si>
   <si>
-    <t>zhuge_bow_icon</t>
-  </si>
-  <si>
     <t>zhuge_bow_icon_big</t>
   </si>
   <si>
-    <t>zhuge_bow吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>multi_bow</t>
   </si>
   <si>
-    <t>multi_bow_icon</t>
-  </si>
-  <si>
     <t>multi_bow_icon_big</t>
   </si>
   <si>
-    <t>multi_bow吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>hand_bow</t>
   </si>
   <si>
     <t>hand_bow_icon</t>
   </si>
   <si>
-    <t>hand_bow吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>shadow_charm</t>
   </si>
   <si>
     <t>shadow_charm_icon</t>
   </si>
   <si>
-    <t>shadow_charm吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>exchange_charm</t>
   </si>
   <si>
     <t>exchange_charm_icon</t>
   </si>
   <si>
-    <t>exchange_charm吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>silent_charm</t>
   </si>
   <si>
     <t>silent_charm_icon</t>
   </si>
   <si>
-    <t>silent_charm吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>confine_charm</t>
   </si>
   <si>
     <t>confine_charm_icon</t>
   </si>
   <si>
-    <t>confine_charm吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>thunder_charm</t>
   </si>
   <si>
     <t>thunder_charm_icon</t>
   </si>
   <si>
-    <t>thunder_charm吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>energy_potion</t>
   </si>
   <si>
-    <t>energy_potion_icon</t>
-  </si>
-  <si>
-    <t>energy_potion吧啦吧啦吧啦吧啦吧啦吧啦</t>
-  </si>
-  <si>
     <t>angry_potion</t>
-  </si>
-  <si>
-    <t>angry_potion_icon</t>
-  </si>
-  <si>
-    <t>angry_potion吧啦吧啦吧啦吧啦吧啦吧啦</t>
   </si>
 </sst>
 </file>
@@ -933,7 +831,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -945,6 +843,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1471,43 +1372,38 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AC20"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="4.70192307692308" customWidth="1"/>
-    <col min="2" max="2" width="5.39423076923077" customWidth="1"/>
-    <col min="3" max="3" width="10.4423076923077" customWidth="1"/>
+    <col min="2" max="3" width="10.4423076923077" customWidth="1"/>
     <col min="4" max="4" width="10.5865384615385" customWidth="1"/>
-    <col min="5" max="6" width="14.6730769230769" customWidth="1"/>
-    <col min="7" max="7" width="19.5961538461538" customWidth="1"/>
-    <col min="8" max="8" width="20.8269230769231" customWidth="1"/>
-    <col min="9" max="9" width="11.2115384615385" customWidth="1"/>
-    <col min="10" max="10" width="10.4807692307692" customWidth="1"/>
-    <col min="11" max="11" width="15.8942307692308" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.3653846153846" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6730769230769" customWidth="1"/>
+    <col min="6" max="7" width="20.8269230769231" customWidth="1"/>
+    <col min="8" max="8" width="11.2115384615385" customWidth="1"/>
+    <col min="9" max="9" width="10.4807692307692" customWidth="1"/>
+    <col min="10" max="10" width="15.8942307692308" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.3653846153846" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.3653846153846" customWidth="1"/>
     <col min="13" max="13" width="18.3653846153846" customWidth="1"/>
     <col min="14" max="14" width="18.4903846153846" customWidth="1"/>
     <col min="15" max="15" width="11.5769230769231" customWidth="1"/>
     <col min="16" max="16" width="16.0192307692308" customWidth="1"/>
-    <col min="17" max="18" width="18.4807692307692" customWidth="1"/>
-    <col min="19" max="19" width="18.6057692307692" customWidth="1"/>
-    <col min="20" max="20" width="11.7019230769231" customWidth="1"/>
-    <col min="21" max="21" width="16.1442307692308" customWidth="1"/>
-    <col min="22" max="23" width="18.7307692307692" customWidth="1"/>
-    <col min="24" max="24" width="18.8653846153846" customWidth="1"/>
-    <col min="25" max="25" width="11.7019230769231" customWidth="1"/>
-    <col min="26" max="26" width="70.5" customWidth="1"/>
-    <col min="27" max="27" width="12.0769230769231" customWidth="1"/>
-    <col min="28" max="28" width="12.5673076923077" customWidth="1"/>
-    <col min="29" max="29" width="12.3173076923077" customWidth="1"/>
+    <col min="17" max="19" width="18.4807692307692" customWidth="1"/>
+    <col min="20" max="20" width="18.6057692307692" customWidth="1"/>
+    <col min="21" max="21" width="11.7019230769231" customWidth="1"/>
+    <col min="22" max="22" width="16.1442307692308" customWidth="1"/>
+    <col min="23" max="25" width="18.7307692307692" customWidth="1"/>
+    <col min="26" max="26" width="18.8653846153846" customWidth="1"/>
+    <col min="27" max="27" width="11.7019230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1529,13 +1425,13 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1559,7 +1455,7 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
@@ -1577,7 +1473,7 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Y1" t="s">
@@ -1589,19 +1485,13 @@
       <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -1612,26 +1502,26 @@
       <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
         <v>3</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
       <c r="K2" s="1">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
       <c r="M2">
         <v>-1</v>
@@ -1639,25 +1529,13 @@
       <c r="O2">
         <v>10</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA2">
-        <v>-1</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:15">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1668,26 +1546,26 @@
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>33</v>
+      <c r="F3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
         <v>3</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3" s="1">
-        <v>3</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
       </c>
       <c r="M3">
         <v>-1</v>
@@ -1695,25 +1573,13 @@
       <c r="O3">
         <v>20</v>
       </c>
-      <c r="Z3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA3">
-        <v>-1</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" ht="17" customHeight="1" spans="1:29">
+    <row r="4" ht="17" customHeight="1" spans="1:15">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>2</v>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1724,26 +1590,26 @@
       <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>37</v>
+      <c r="F4" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
       </c>
       <c r="K4" s="1">
-        <v>3</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
       </c>
       <c r="M4">
         <v>-1</v>
@@ -1751,25 +1617,13 @@
       <c r="O4">
         <v>30</v>
       </c>
-      <c r="Z4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA4">
-        <v>-1</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:15">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>33</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1780,26 +1634,26 @@
       <c r="E5" s="2">
         <v>-1</v>
       </c>
-      <c r="F5" t="s">
-        <v>41</v>
+      <c r="F5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
       </c>
       <c r="I5">
-        <v>-1</v>
-      </c>
-      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
         <v>0</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="L5" s="1">
-        <v>0</v>
+      <c r="L5">
+        <v>1</v>
       </c>
       <c r="M5">
         <v>7</v>
@@ -1807,25 +1661,13 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="Z5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA5">
-        <v>-1</v>
-      </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:15">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>35</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -1836,26 +1678,26 @@
       <c r="E6" s="2">
         <v>-1</v>
       </c>
-      <c r="F6" t="s">
-        <v>45</v>
+      <c r="F6" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="H6">
+        <v>-1</v>
       </c>
       <c r="I6">
-        <v>-1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="1">
-        <v>0</v>
+      <c r="L6">
+        <v>1</v>
       </c>
       <c r="M6">
         <v>11</v>
@@ -1863,25 +1705,13 @@
       <c r="O6">
         <v>30</v>
       </c>
-      <c r="Z6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA6">
-        <v>-1</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:15">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>37</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1892,26 +1722,26 @@
       <c r="E7" s="2">
         <v>-1</v>
       </c>
-      <c r="F7" t="s">
-        <v>49</v>
+      <c r="F7" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
       </c>
       <c r="I7">
-        <v>-1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
-      <c r="L7" s="1">
-        <v>0</v>
+      <c r="L7">
+        <v>1</v>
       </c>
       <c r="M7">
         <v>11</v>
@@ -1919,25 +1749,13 @@
       <c r="O7">
         <v>20</v>
       </c>
-      <c r="Z7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA7">
-        <v>-1</v>
-      </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-      <c r="AC7">
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:15">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>39</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1948,26 +1766,26 @@
       <c r="E8" s="2">
         <v>-1</v>
       </c>
-      <c r="F8" t="s">
-        <v>53</v>
+      <c r="F8" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
+        <v>40</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
       </c>
       <c r="I8">
-        <v>-1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="L8" s="1">
-        <v>0</v>
+      <c r="L8">
+        <v>1</v>
       </c>
       <c r="M8">
         <v>11</v>
@@ -1975,25 +1793,13 @@
       <c r="O8">
         <v>10</v>
       </c>
-      <c r="Z8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA8">
-        <v>-1</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:15">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>1</v>
+      <c r="B9" t="s">
+        <v>41</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -2004,26 +1810,26 @@
       <c r="E9" s="2">
         <v>-1</v>
       </c>
-      <c r="F9" t="s">
-        <v>57</v>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
+        <v>42</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
       </c>
       <c r="K9" s="1">
-        <v>3</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
       <c r="M9">
         <v>-1</v>
@@ -2031,25 +1837,13 @@
       <c r="O9">
         <v>15</v>
       </c>
-      <c r="Z9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA9">
-        <v>-1</v>
-      </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-      <c r="AC9">
-        <v>1</v>
-      </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:15">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" t="s">
+        <v>43</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2060,26 +1854,26 @@
       <c r="E10" s="2">
         <v>-1</v>
       </c>
-      <c r="F10" t="s">
-        <v>61</v>
+      <c r="F10" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>1</v>
+      <c r="J10" s="1">
+        <v>3</v>
       </c>
       <c r="K10" s="1">
-        <v>3</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
       </c>
       <c r="M10">
         <v>-1</v>
@@ -2087,25 +1881,13 @@
       <c r="O10">
         <v>10</v>
       </c>
-      <c r="Z10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA10">
-        <v>-1</v>
-      </c>
-      <c r="AB10">
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <v>1</v>
-      </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:15">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>2</v>
+      <c r="B11" t="s">
+        <v>45</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -2116,26 +1898,26 @@
       <c r="E11" s="2">
         <v>-1</v>
       </c>
-      <c r="F11" t="s">
-        <v>65</v>
+      <c r="F11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
       </c>
       <c r="K11" s="1">
-        <v>3</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
       </c>
       <c r="M11">
         <v>-1</v>
@@ -2143,34 +1925,13 @@
       <c r="O11">
         <v>10</v>
       </c>
-      <c r="P11">
-        <v>3</v>
-      </c>
-      <c r="R11">
-        <v>-1</v>
-      </c>
-      <c r="T11">
-        <v>10</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA11">
-        <v>-1</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>1</v>
-      </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:15">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>1</v>
+      <c r="B12" t="s">
+        <v>47</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2181,26 +1942,26 @@
       <c r="E12" s="2">
         <v>-1</v>
       </c>
-      <c r="F12" t="s">
-        <v>69</v>
+      <c r="F12" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" t="s">
-        <v>71</v>
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>4</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3</v>
       </c>
       <c r="K12" s="1">
-        <v>3</v>
-      </c>
-      <c r="L12" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
       </c>
       <c r="M12">
         <v>-1</v>
@@ -2208,34 +1969,13 @@
       <c r="O12">
         <v>6</v>
       </c>
-      <c r="P12">
-        <v>3</v>
-      </c>
-      <c r="R12">
-        <v>-1</v>
-      </c>
-      <c r="T12">
-        <v>6</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA12">
-        <v>-1</v>
-      </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
-      <c r="AC12">
-        <v>1</v>
-      </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:15">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" t="s">
+        <v>49</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2246,26 +1986,26 @@
       <c r="E13" s="2">
         <v>-1</v>
       </c>
-      <c r="F13" t="s">
-        <v>73</v>
+      <c r="F13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" t="s">
-        <v>74</v>
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
       </c>
       <c r="I13">
-        <v>4</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3</v>
       </c>
       <c r="K13" s="1">
-        <v>3</v>
-      </c>
-      <c r="L13" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
       </c>
       <c r="M13">
         <v>-1</v>
@@ -2273,25 +2013,13 @@
       <c r="O13">
         <v>10</v>
       </c>
-      <c r="Z13" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA13">
-        <v>-1</v>
-      </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <v>1</v>
-      </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:15">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>1</v>
+      <c r="B14" t="s">
+        <v>51</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2302,49 +2030,37 @@
       <c r="E14" s="2">
         <v>-1</v>
       </c>
-      <c r="F14" t="s">
-        <v>76</v>
+      <c r="F14" t="b">
+        <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H14" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="H14">
+        <v>-1</v>
       </c>
       <c r="I14">
-        <v>-1</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
       </c>
       <c r="K14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
-      <c r="Z14" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA14">
-        <v>-1</v>
-      </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>1</v>
-      </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:12">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>1</v>
+      <c r="B15" t="s">
+        <v>53</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2355,46 +2071,34 @@
       <c r="E15" s="2">
         <v>-1</v>
       </c>
-      <c r="F15" t="s">
-        <v>79</v>
+      <c r="F15" t="b">
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>80</v>
+        <v>54</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
       </c>
       <c r="I15">
-        <v>5</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2</v>
       </c>
       <c r="K15" s="1">
-        <v>2</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA15">
-        <v>-1</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:15">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" t="s">
+        <v>55</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2405,49 +2109,37 @@
       <c r="E16" s="2">
         <v>-1</v>
       </c>
-      <c r="F16" t="s">
-        <v>82</v>
+      <c r="F16" t="b">
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
-      </c>
-      <c r="H16" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
       </c>
       <c r="I16">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
       </c>
       <c r="O16">
         <v>12</v>
       </c>
-      <c r="Z16" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA16">
-        <v>-1</v>
-      </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <v>1</v>
-      </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:15">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" t="s">
+        <v>57</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2458,49 +2150,37 @@
       <c r="E17" s="2">
         <v>-1</v>
       </c>
-      <c r="F17" t="s">
-        <v>85</v>
+      <c r="F17" t="b">
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" t="s">
-        <v>86</v>
+        <v>58</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
       </c>
       <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
       </c>
       <c r="O17">
         <v>13</v>
       </c>
-      <c r="Z17" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA17">
-        <v>-1</v>
-      </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
-      <c r="AC17">
-        <v>1</v>
-      </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:15">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>59</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2511,26 +2191,26 @@
       <c r="E18" s="2">
         <v>-1</v>
       </c>
-      <c r="F18" t="s">
-        <v>88</v>
+      <c r="F18" t="b">
+        <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" t="s">
-        <v>89</v>
+        <v>60</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
       </c>
       <c r="I18">
-        <v>4</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3</v>
       </c>
       <c r="K18" s="1">
-        <v>3</v>
-      </c>
-      <c r="L18" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
       </c>
       <c r="M18">
         <v>-1</v>
@@ -2538,52 +2218,40 @@
       <c r="O18">
         <v>20</v>
       </c>
-      <c r="Z18" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA18">
-        <v>-1</v>
-      </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-      <c r="AC18">
-        <v>1</v>
-      </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:15">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>1</v>
+      <c r="B19" t="s">
+        <v>61</v>
       </c>
       <c r="C19">
         <v>-1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2">
         <v>-1</v>
       </c>
-      <c r="F19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" t="s">
-        <v>92</v>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>-1</v>
       </c>
       <c r="I19">
-        <v>-1</v>
-      </c>
-      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
         <v>0</v>
       </c>
       <c r="K19" s="1">
         <v>0</v>
       </c>
-      <c r="L19" s="1">
-        <v>0</v>
+      <c r="L19">
+        <v>1</v>
       </c>
       <c r="M19">
         <v>7</v>
@@ -2591,70 +2259,46 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="Z19" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA19">
-        <v>-1</v>
-      </c>
-      <c r="AB19">
-        <v>0</v>
-      </c>
-      <c r="AC19">
-        <v>1</v>
-      </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:15">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>1</v>
+      <c r="B20" t="s">
+        <v>62</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20" s="2">
         <v>-1</v>
       </c>
-      <c r="F20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>-1</v>
       </c>
       <c r="I20">
-        <v>-1</v>
-      </c>
-      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
       </c>
-      <c r="L20" s="1">
-        <v>0</v>
+      <c r="L20">
+        <v>1</v>
       </c>
       <c r="M20">
         <v>10</v>
       </c>
       <c r="O20">
         <v>150</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA20">
-        <v>-1</v>
-      </c>
-      <c r="AB20">
-        <v>0</v>
-      </c>
-      <c r="AC20">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Item Use logic & add battle effect
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13160"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2095,7 +2095,7 @@
         <v>100</v>
       </c>
       <c r="K14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L14" s="1">
         <v>0</v>
@@ -2142,7 +2142,7 @@
         <v>100</v>
       </c>
       <c r="K15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="1">
         <v>0</v>
@@ -2186,7 +2186,7 @@
         <v>100</v>
       </c>
       <c r="K16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" s="1">
         <v>0</v>
@@ -2233,7 +2233,7 @@
         <v>100</v>
       </c>
       <c r="K17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
better logic & bug fix
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="28800" windowHeight="13160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>

<commit_message>
common enemy ai & bugs fix
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="28800" windowHeight="13160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <t>effect1.invokeType</t>
   </si>
   <si>
-    <t>effect1.invokeNum</t>
+    <t>effect1.invokeTime</t>
   </si>
   <si>
     <t>effect1.propertyType</t>
@@ -1389,8 +1389,8 @@
   <sheetPr/>
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1548,7 +1548,9 @@
       <c r="K2">
         <v>10</v>
       </c>
-      <c r="L2"/>
+      <c r="L2">
+        <v>0</v>
+      </c>
       <c r="M2" s="1">
         <v>3</v>
       </c>
@@ -1599,7 +1601,9 @@
       <c r="K3">
         <v>20</v>
       </c>
-      <c r="L3"/>
+      <c r="L3">
+        <v>0</v>
+      </c>
       <c r="M3" s="1">
         <v>3</v>
       </c>
@@ -1650,7 +1654,9 @@
       <c r="K4">
         <v>30</v>
       </c>
-      <c r="L4"/>
+      <c r="L4">
+        <v>0</v>
+      </c>
       <c r="M4" s="1">
         <v>3</v>
       </c>
@@ -1701,7 +1707,9 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5"/>
+      <c r="L5">
+        <v>0</v>
+      </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
@@ -1911,7 +1919,9 @@
       <c r="K9">
         <v>15</v>
       </c>
-      <c r="L9"/>
+      <c r="L9">
+        <v>0</v>
+      </c>
       <c r="M9" s="1">
         <v>3</v>
       </c>
@@ -1962,7 +1972,9 @@
       <c r="K10">
         <v>10</v>
       </c>
-      <c r="L10"/>
+      <c r="L10">
+        <v>0</v>
+      </c>
       <c r="M10" s="1">
         <v>3</v>
       </c>
@@ -2013,7 +2025,9 @@
       <c r="K11">
         <v>20</v>
       </c>
-      <c r="L11"/>
+      <c r="L11">
+        <v>0</v>
+      </c>
       <c r="M11" s="1">
         <v>3</v>
       </c>
@@ -2064,7 +2078,9 @@
       <c r="K12">
         <v>12</v>
       </c>
-      <c r="L12"/>
+      <c r="L12">
+        <v>0</v>
+      </c>
       <c r="M12" s="1">
         <v>3</v>
       </c>
@@ -2115,7 +2131,9 @@
       <c r="K13">
         <v>10</v>
       </c>
-      <c r="L13"/>
+      <c r="L13">
+        <v>0</v>
+      </c>
       <c r="M13" s="1">
         <v>3</v>
       </c>
@@ -2166,7 +2184,9 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14"/>
+      <c r="L14">
+        <v>0</v>
+      </c>
       <c r="M14" s="1">
         <v>2</v>
       </c>
@@ -2217,7 +2237,9 @@
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15"/>
+      <c r="L15">
+        <v>0</v>
+      </c>
       <c r="M15" s="1">
         <v>1</v>
       </c>
@@ -2265,7 +2287,9 @@
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16"/>
+      <c r="L16">
+        <v>0</v>
+      </c>
       <c r="M16" s="1">
         <v>2</v>
       </c>
@@ -2316,7 +2340,9 @@
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17"/>
+      <c r="L17">
+        <v>0</v>
+      </c>
       <c r="M17" s="1">
         <v>2</v>
       </c>
@@ -2367,7 +2393,9 @@
       <c r="K18">
         <v>20</v>
       </c>
-      <c r="L18"/>
+      <c r="L18">
+        <v>0</v>
+      </c>
       <c r="M18" s="1">
         <v>3</v>
       </c>
@@ -2415,7 +2443,9 @@
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19"/>
+      <c r="L19">
+        <v>0</v>
+      </c>
       <c r="M19" s="1">
         <v>0</v>
       </c>
@@ -2463,7 +2493,9 @@
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20"/>
+      <c r="L20">
+        <v>0</v>
+      </c>
       <c r="M20" s="1">
         <v>0</v>
       </c>
@@ -2512,9 +2544,11 @@
         <v>100</v>
       </c>
       <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21"/>
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
       <c r="M21" s="1">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
bag window food bug fixes
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13160"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1389,8 +1389,8 @@
   <sheetPr/>
   <dimension ref="A1:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2420,7 +2420,7 @@
         <v>64</v>
       </c>
       <c r="C19">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2470,7 +2470,7 @@
         <v>65</v>
       </c>
       <c r="C20">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>

</xml_diff>

<commit_message>
new property & time past logic & five elements chart
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>elementsType</t>
   </si>
   <si>
     <t>equipType</t>
@@ -1387,42 +1390,43 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AD21"/>
+  <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:R1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="4.70192307692308" customWidth="1"/>
     <col min="2" max="2" width="13.1826923076923" customWidth="1"/>
-    <col min="3" max="3" width="10.4423076923077" customWidth="1"/>
-    <col min="4" max="4" width="10.5865384615385" customWidth="1"/>
-    <col min="5" max="5" width="14.6730769230769" customWidth="1"/>
-    <col min="6" max="6" width="20.8269230769231" customWidth="1"/>
-    <col min="7" max="7" width="24.0384615384615" customWidth="1"/>
-    <col min="8" max="8" width="11.2115384615385" customWidth="1"/>
-    <col min="9" max="9" width="10.4807692307692" customWidth="1"/>
-    <col min="10" max="10" width="15.8942307692308" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.9038461538462" customWidth="1"/>
-    <col min="12" max="12" width="13.9326923076923" customWidth="1"/>
-    <col min="13" max="13" width="15.8942307692308" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.3653846153846" style="1" customWidth="1"/>
-    <col min="15" max="16" width="18.3653846153846" customWidth="1"/>
-    <col min="17" max="17" width="18.4903846153846" customWidth="1"/>
-    <col min="18" max="18" width="11.5769230769231" customWidth="1"/>
-    <col min="19" max="19" width="16.0192307692308" customWidth="1"/>
-    <col min="20" max="22" width="18.4807692307692" customWidth="1"/>
-    <col min="23" max="23" width="18.6057692307692" customWidth="1"/>
-    <col min="24" max="24" width="11.7019230769231" customWidth="1"/>
-    <col min="25" max="25" width="16.1442307692308" customWidth="1"/>
-    <col min="26" max="28" width="18.7307692307692" customWidth="1"/>
-    <col min="29" max="29" width="18.8653846153846" customWidth="1"/>
-    <col min="30" max="30" width="11.7019230769231" customWidth="1"/>
+    <col min="3" max="3" width="14.6634615384615" customWidth="1"/>
+    <col min="4" max="4" width="10.4423076923077" customWidth="1"/>
+    <col min="5" max="5" width="10.5865384615385" customWidth="1"/>
+    <col min="6" max="6" width="14.6730769230769" customWidth="1"/>
+    <col min="7" max="7" width="20.8269230769231" customWidth="1"/>
+    <col min="8" max="8" width="24.0384615384615" customWidth="1"/>
+    <col min="9" max="9" width="11.2115384615385" customWidth="1"/>
+    <col min="10" max="10" width="10.4807692307692" customWidth="1"/>
+    <col min="11" max="11" width="15.8942307692308" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.9038461538462" customWidth="1"/>
+    <col min="13" max="13" width="13.9326923076923" customWidth="1"/>
+    <col min="14" max="14" width="15.8942307692308" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.3653846153846" style="1" customWidth="1"/>
+    <col min="16" max="17" width="18.3653846153846" customWidth="1"/>
+    <col min="18" max="18" width="18.4903846153846" customWidth="1"/>
+    <col min="19" max="19" width="11.5769230769231" customWidth="1"/>
+    <col min="20" max="20" width="16.0192307692308" customWidth="1"/>
+    <col min="21" max="23" width="18.4807692307692" customWidth="1"/>
+    <col min="24" max="24" width="18.6057692307692" customWidth="1"/>
+    <col min="25" max="25" width="11.7019230769231" customWidth="1"/>
+    <col min="26" max="26" width="16.1442307692308" customWidth="1"/>
+    <col min="27" max="29" width="18.7307692307692" customWidth="1"/>
+    <col min="30" max="30" width="18.8653846153846" customWidth="1"/>
+    <col min="31" max="31" width="11.7019230769231" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1444,22 +1448,22 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1468,7 +1472,7 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" t="s">
@@ -1483,10 +1487,10 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
@@ -1501,10 +1505,10 @@
       <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AC1" t="s">
@@ -1513,1055 +1517,1118 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
       <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2">
         <v>3</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
         <v>100</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>10</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <v>3</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
+      <c r="O2" s="1">
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>-1</v>
-      </c>
-      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>-1</v>
+      </c>
+      <c r="S2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>100</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>20</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
         <v>3</v>
       </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
+      <c r="O3" s="1">
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>-1</v>
-      </c>
-      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>-1</v>
+      </c>
+      <c r="S3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" ht="17" customHeight="1" spans="1:18">
+    <row r="4" ht="17" customHeight="1" spans="1:19">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4">
         <v>4</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
         <v>100</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>30</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
         <v>3</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
+      <c r="O4" s="1">
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>-1</v>
-      </c>
-      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>-1</v>
+      </c>
+      <c r="S4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
         <v>100</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
-      <c r="O5">
-        <v>1</v>
+      <c r="O5" s="1">
+        <v>0</v>
       </c>
       <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>7</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6">
-        <v>-1</v>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
       </c>
       <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
         <v>100</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>30</v>
       </c>
-      <c r="M6" s="1">
-        <v>0</v>
-      </c>
       <c r="N6" s="1">
         <v>0</v>
       </c>
-      <c r="O6">
-        <v>1</v>
+      <c r="O6" s="1">
+        <v>0</v>
       </c>
       <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
         <v>11</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7">
-        <v>-1</v>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
       </c>
       <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
         <v>100</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
       <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>20</v>
       </c>
-      <c r="M7" s="1">
-        <v>0</v>
-      </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
-      <c r="O7">
-        <v>1</v>
+      <c r="O7" s="1">
+        <v>0</v>
       </c>
       <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
         <v>11</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F8" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8">
-        <v>-1</v>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
       </c>
       <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
         <v>100</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>10</v>
       </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
       <c r="N8" s="1">
         <v>0</v>
       </c>
-      <c r="O8">
-        <v>1</v>
+      <c r="O8" s="1">
+        <v>0</v>
       </c>
       <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
         <v>11</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9">
         <v>2</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1">
         <v>100</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>15</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
         <v>3</v>
       </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
+      <c r="O9" s="1">
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>-1</v>
-      </c>
-      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>-1</v>
+      </c>
+      <c r="S9">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
         <v>100</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>10</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
         <v>3</v>
       </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
+      <c r="O10" s="1">
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>-1</v>
-      </c>
-      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>-1</v>
+      </c>
+      <c r="S10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11">
         <v>5</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
         <v>100</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>20</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="1">
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
         <v>3</v>
       </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11">
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>2</v>
       </c>
-      <c r="P11">
-        <v>-1</v>
-      </c>
-      <c r="R11">
+      <c r="Q11">
+        <v>-1</v>
+      </c>
+      <c r="S11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12">
         <v>4</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
         <v>100</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>12</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1">
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
         <v>3</v>
       </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12">
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>2</v>
       </c>
-      <c r="P12">
-        <v>-1</v>
-      </c>
-      <c r="R12">
+      <c r="Q12">
+        <v>-1</v>
+      </c>
+      <c r="S12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13">
         <v>4</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
         <v>100</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>10</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1">
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
         <v>3</v>
       </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
+      <c r="O13" s="1">
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>-1</v>
-      </c>
-      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>-1</v>
+      </c>
+      <c r="S13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-1</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14">
-        <v>-1</v>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>56</v>
       </c>
       <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
         <v>100</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
         <v>2</v>
       </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
+      <c r="O14" s="1">
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>-1</v>
-      </c>
-      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>-1</v>
+      </c>
+      <c r="S14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15">
         <v>5</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
         <v>100</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" s="1">
-        <v>1</v>
+      <c r="M15">
+        <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
       </c>
       <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-1</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16">
         <v>4</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
         <v>100</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
         <v>2</v>
       </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
+      <c r="O16" s="1">
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>-1</v>
-      </c>
-      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>-1</v>
+      </c>
+      <c r="S16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:19">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-1</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17">
         <v>4</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
         <v>100</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
         <v>2</v>
       </c>
-      <c r="N17" s="1">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
+      <c r="O17" s="1">
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>-1</v>
-      </c>
-      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>-1</v>
+      </c>
+      <c r="S17">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:19">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-1</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18">
         <v>4</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
         <v>100</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>20</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1">
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
         <v>3</v>
       </c>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
+      <c r="O18" s="1">
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>-1</v>
-      </c>
-      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>-1</v>
+      </c>
+      <c r="S18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:19">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-1</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>-1</v>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
         <v>100</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
-      <c r="O19">
-        <v>1</v>
+      <c r="O19" s="1">
+        <v>0</v>
       </c>
       <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
         <v>7</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:19">
       <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-1</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" s="2">
-        <v>-1</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>-1</v>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
         <v>100</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
       </c>
-      <c r="O20">
-        <v>1</v>
+      <c r="O20" s="1">
+        <v>0</v>
       </c>
       <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
         <v>10</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21">
+        <v>67</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21">
         <v>4</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1">
         <v>100</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>10</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1">
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
         <v>3</v>
       </c>
-      <c r="N21" s="1">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
+      <c r="O21" s="1">
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>-1</v>
-      </c>
-      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>-1</v>
+      </c>
+      <c r="S21">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
five elements type display
equip & team window display improve
</commit_message>
<xml_diff>
--- a/Data/EquipDefine.xlsx
+++ b/Data/EquipDefine.xlsx
@@ -35,7 +35,7 @@
     <t>title</t>
   </si>
   <si>
-    <t>elementsType</t>
+    <t>fiveElementsType</t>
   </si>
   <si>
     <t>equipType</t>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>

</xml_diff>